<commit_message>
Testng with DataProvider changes today
</commit_message>
<xml_diff>
--- a/dataFiles/data.xlsx
+++ b/dataFiles/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Radhika\Test Leaf\Sel\SeleniumRedoBootCamp\dataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0F80FF-EAA0-44B2-AC5D-D2FA3D5BCA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FD9FA1-3438-404D-A38C-3C3726618933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{846CCA41-D9C2-483C-B839-FEBE7D653030}"/>
   </bookViews>
@@ -412,7 +412,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>